<commit_message>
Modified Original Course Code
</commit_message>
<xml_diff>
--- a/Comandos_CMD.xlsx
+++ b/Comandos_CMD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AllisonAponte\Documents\Education\Coursera\RubyOnRails\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AllisonAponte\Documents\Education\Coursera\Ruby_On_Rails\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
   <si>
     <t>reinicia</t>
   </si>
@@ -365,6 +365,21 @@
   </si>
   <si>
     <t>Create a new repository on the command line</t>
+  </si>
+  <si>
+    <t>git fork</t>
+  </si>
+  <si>
+    <t>means you are copying the repository to your Github account</t>
+  </si>
+  <si>
+    <t>means you are returning the repository after modifying it</t>
+  </si>
+  <si>
+    <t>means you are making a copy of the repository in your system == DOWNLOADING</t>
+  </si>
+  <si>
+    <t>means you are fetching the last modified repository == REFRESHING</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,6 +1253,38 @@
       </c>
       <c r="B17" s="1" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>